<commit_message>
sprint 107 Recipes testcases
</commit_message>
<xml_diff>
--- a/Buyer hub/Recipes/Current sprint testcases/Recipes Listing page.xlsx
+++ b/Buyer hub/Recipes/Current sprint testcases/Recipes Listing page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Recipes\Current sprint testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F48B7D-BDBA-4330-84AB-BB3CFE1B9CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE13B81-C657-435D-8549-0EA83CAD2174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>SL. No</t>
   </si>
@@ -93,6 +93,181 @@
     <t>Recipes menu page</t>
   </si>
   <si>
+    <t>Click the Recipes &gt; Outlets</t>
+  </si>
+  <si>
+    <t>Select the particular outlet</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select the particular </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Outlet &gt; Delete</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select the particular </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Outlet &gt; Settings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Recipe by selecting the checkbox next to the recipe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">when </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Settings </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is clicked, User can set the 'ideal' food cost percentage.by default this is already set at 22%</t>
+    </r>
+  </si>
+  <si>
+    <t>Create Recipe page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Create the page and click the Copy data from          2.Copy data from dropdown ,select the Recipe      </t>
+  </si>
+  <si>
+    <t>User can copy data from another recipe or sub-recipe in the same outlet using the "Copy recipe from" button. It will completely overwrite any existing data on the page</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Recipe page &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cost per portion</t>
+    </r>
+  </si>
+  <si>
+    <t>Once click the Cost per portion It shows details</t>
+  </si>
+  <si>
+    <t>Select the Item from the dropdown and Quantity to use, UOM and Save</t>
+  </si>
+  <si>
+    <r>
+      <t>Create Recipe page &gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add ingredient</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Recipe page &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UOM</t>
+    </r>
+  </si>
+  <si>
+    <t>If he needs to use a specific UOM that does not already have the conversation rate information</t>
+  </si>
+  <si>
+    <t>If non-inventory SKUs are added to a recipe, user will be prompted to add the item to an inventory list first. They can also create a new inventory list from this step (in case the outlet has not set up inventory at all). The item will be added to inventory using the UOM selected in this recipe.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Recipe page &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select inventory list dropdown</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1.Once click the Recipes menu it should shows the </t>
     </r>
@@ -115,7 +290,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> linked to the user.                               2.Next to every outlet, we display the number of </t>
+      <t xml:space="preserve"> linked to the user.                                            2.Next to every outlet, we display the number of </t>
     </r>
     <r>
       <rPr>
@@ -130,106 +305,7 @@
     </r>
   </si>
   <si>
-    <t>Click the Recipes &gt; Outlets</t>
-  </si>
-  <si>
-    <t>Select the particular outlet</t>
-  </si>
-  <si>
-    <t>1.It shows On Top left outlet name, right settings and Create new                                                                        2.Name, Cost, Retail price and Cost%</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Select the particular </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Outlet &gt; Delete</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Select the particular </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Outlet &gt; Settings</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">User can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delete</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Recipe by selecting the checkbox next to the recipe</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">when </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Settings </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is clicked, User can set the 'ideal' food cost percentage.by default this is already set at 22%</t>
-    </r>
-  </si>
-  <si>
-    <t>Create Recipe page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Create the page and click the Copy data from          2.Copy data from dropdown ,select the Recipe      </t>
-  </si>
-  <si>
-    <t>User can copy data from another recipe or sub-recipe in the same outlet using the "Copy recipe from" button. It will completely overwrite any existing data on the page</t>
+    <t>1.It shows On Top left outlet name, right settings and Create new                                                                                           2.Name, Cost, Retail price and Cost%</t>
   </si>
   <si>
     <r>
@@ -244,56 +320,165 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Cost per portion</t>
-    </r>
-  </si>
-  <si>
-    <t>Once click the Cost per portion It shows details</t>
-  </si>
-  <si>
-    <t>Select the Item from the dropdown and Quantity to use, UOM and Save</t>
-  </si>
-  <si>
-    <r>
-      <t>Create Recipe page &gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Add ingredient</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create Recipe page &gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UOM</t>
-    </r>
-  </si>
-  <si>
-    <t>If he needs to use a specific UOM that does not already have the conversation rate information</t>
+      <t>Select inventory list dropdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; New inventory list</t>
+    </r>
+  </si>
+  <si>
+    <t>Create the List name and Save</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Sub recipe &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select inventory list dropdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; New inventory list</t>
+    </r>
+  </si>
+  <si>
+    <t>User can convert a recipe page into a sub-recipe by selecting the "This is a sub-recipe" checkbox below the "Recipe name" field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In "Inventory", user will see an error when trying to remove from Inventory an SKU still used in recipes. They’ll need to remove this SKU from recipes first.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When viewing a previously a created recipe, the page is exactly the same as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Create recipe"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, but there is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Delete"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button and a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"last updated"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> timestamp at the top.</t>
+    </r>
+  </si>
+  <si>
+    <t>Inventory page</t>
+  </si>
+  <si>
+    <t>Click the Outlets &gt; SKU</t>
+  </si>
+  <si>
+    <t>In inventory when trying to remove from inventory</t>
+  </si>
+  <si>
+    <t>Particular SKU &gt; Settings page (tap on SKU)</t>
+  </si>
+  <si>
+    <t>If the item is an ingredient in recipes, a warning appears when user changes the inventory UOM to something else. The inventory UOM used in the recipes will be changed to the new inventory UOM but the quantity used in the recipes will not change.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +503,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF172B4D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -393,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -421,6 +620,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +919,7 @@
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" customWidth="1"/>
     <col min="4" max="4" width="44.140625" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
     <col min="6" max="6" width="42.28515625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
@@ -819,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -831,13 +1037,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -848,13 +1054,13 @@
         <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,13 +1071,13 @@
         <v>21</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -882,16 +1088,16 @@
         <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -902,13 +1108,13 @@
         <v>21</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -919,13 +1125,13 @@
         <v>21</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -936,13 +1142,115 @@
         <v>21</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="131.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>38</v>
+    </row>
+    <row r="14" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>